<commit_message>
parallel process adapter removal
</commit_message>
<xml_diff>
--- a/utils/index_list.xlsx
+++ b/utils/index_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krdav/Google Drive/MCB/Sullivan_lab/tRNA-charge-seq/1-fastq_processing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krdav/Google Drive/MCB/Sullivan_lab/tRNA-charge-seq/utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E76C52C-3A63-344A-B627-E6B24720A6AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE31F279-A06D-5847-9EFD-0407368E5B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="6460" windowWidth="27040" windowHeight="11540" xr2:uid="{74EA7424-48A6-C04A-A5DF-8688B5191606}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>type</t>
   </si>
@@ -54,18 +54,6 @@
     <t>barcode</t>
   </si>
   <si>
-    <t>l1</t>
-  </si>
-  <si>
-    <t>l2</t>
-  </si>
-  <si>
-    <t>l3</t>
-  </si>
-  <si>
-    <t>l4</t>
-  </si>
-  <si>
     <t>D701</t>
   </si>
   <si>
@@ -96,18 +84,6 @@
     <t>D505</t>
   </si>
   <si>
-    <t>TAAGGCAT</t>
-  </si>
-  <si>
-    <t>CGTACTCG</t>
-  </si>
-  <si>
-    <t>ATGCAGTA</t>
-  </si>
-  <si>
-    <t>GCCTTAGC</t>
-  </si>
-  <si>
     <t>ATTACTCG</t>
   </si>
   <si>
@@ -136,78 +112,6 @@
   </si>
   <si>
     <t>CTTCGCCT</t>
-  </si>
-  <si>
-    <t>l1N</t>
-  </si>
-  <si>
-    <t>l2N</t>
-  </si>
-  <si>
-    <t>l3N</t>
-  </si>
-  <si>
-    <t>l4N</t>
-  </si>
-  <si>
-    <t>TNNNNNNGACTA</t>
-  </si>
-  <si>
-    <t>TNNNNNNAGTGC</t>
-  </si>
-  <si>
-    <t>TNNNNNNTCACG</t>
-  </si>
-  <si>
-    <t>TNNNNNNCTGAT</t>
-  </si>
-  <si>
-    <t>TNNNNNNGCATC</t>
-  </si>
-  <si>
-    <t>TNNNNNNAGCTG</t>
-  </si>
-  <si>
-    <t>TNNNNNNTAGCT</t>
-  </si>
-  <si>
-    <t>TNNNNNNTGCGA</t>
-  </si>
-  <si>
-    <t>TNNNNNNTACAG</t>
-  </si>
-  <si>
-    <t>TNNNNNNCATGA</t>
-  </si>
-  <si>
-    <t>TNNNNNNCTAGC</t>
-  </si>
-  <si>
-    <t>TNNNNNNGTACA</t>
-  </si>
-  <si>
-    <t>l5N</t>
-  </si>
-  <si>
-    <t>l6N</t>
-  </si>
-  <si>
-    <t>l7N</t>
-  </si>
-  <si>
-    <t>l8N</t>
-  </si>
-  <si>
-    <t>l9N</t>
-  </si>
-  <si>
-    <t>l10N</t>
-  </si>
-  <si>
-    <t>l11N</t>
-  </si>
-  <si>
-    <t>l12N</t>
   </si>
   <si>
     <t>l1Sp</t>
@@ -286,7 +190,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -305,12 +209,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -339,11 +237,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,7 +259,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -650,7 +547,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -658,212 +555,202 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D525E1-05CB-A24B-841E-93206D4958F2}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="188" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="142" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -871,10 +758,10 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -882,10 +769,10 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>41</v>
+        <v>33</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -893,10 +780,10 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>42</v>
+        <v>34</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -904,10 +791,10 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -915,10 +802,10 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>44</v>
+        <v>36</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -926,186 +813,10 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" t="s">
-        <v>62</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" t="s">
-        <v>67</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38" t="s">
-        <v>68</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>